<commit_message>
read credentials from properties file
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -12,33 +12,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">1. Test case: Valid input-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Input: Name: John Doe, Email: johndoe@example.com, Password: Password123-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Account created successfully-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Test case: Invalid email format-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Input: Name: Jane Smith, Email: jan[email protected], Password: Password456-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Error message "Invalid email format"+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">1. Test case: Valid registration+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Input: Name: John Doe, Email: johndoe@example.com, Password: test1234+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Account successfully created with the provided details. </t>
   </si>
   <si>
@@ -46,51 +30,63 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">2. Test case: Registration with existing email+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Input: Name: Jane Smith, Email: janesmith@example.com, Password: test5678+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Error message displayed indicating that the email address is already associated with an existing account.+</t>
+  </si>
+  <si>
     <t xml:space="preserve">3. Test case: Weak password </t>
   </si>
   <si>
-    <t xml:space="preserve">  - Input: Name: Alice Johnson, Email: alice.johnson@example.com, Password: abc123-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Error message "Password must be at least 8 characters long and contain a mix of letters, numbers, and special characters"-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Test case: Existing email-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Input: Name: Mark Brown, Email: markbrown@example.com, Password: Password789-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Error message "An account with this email already exists"-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Test case: Special characters in name-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Input: Name: *$%@#^, Email: test@example.com, Password: Test1234-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Account not created, error message "Name can only contain letters and spaces"-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Test case: Long name-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Input: Name: Samantha Elizabeth Johnson, Email: samantha.j@example.com, Password: Test4567-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - Expected result: Account created successfully</t>
+    <t xml:space="preserve">   - Input: Name: Sarah Johnson, Email: sarahjohnson@example.com, Password: 1234+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Error message displayed indicating that the password is too weak and needs to be stronger.+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Test case: Invalid email format+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Input: Name: Michael Brown, Email: michaelbrown123, Password: testpassword+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Error message displayed indicating that the email format is invalid and must be in the correct format.+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Test case: Long name+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Input: Name: Elizabeth Charlotte Victoria Mary Windsor, Email: elizabeth@example.com, Password: test1234+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Account successfully created with the provided details, even with a long name.+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Test case: Empty name field+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Input: Name: "", Email: testuser@example.com, Password: testpassword+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   - Expected outcome: Error message displayed indicating that the name field is required.</t>
   </si>
 </sst>
 </file>
@@ -191,82 +187,82 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>